<commit_message>
Added per output weighting. Merged SingleBlockADS and InMemoryADS to SingleWindowMemoryADS. Refactored Multi_Band_Repair_Marked to use FFT_Equalizer, added comments and better names, and more efficient filtering. Removed deprecated Repair_in_memory.
</commit_message>
<xml_diff>
--- a/docs/nn results 2020.xlsx
+++ b/docs/nn results 2020.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>INPUTS</t>
   </si>
@@ -57,9 +57,6 @@
     <t>10,4k</t>
   </si>
   <si>
-    <t>Weights (negative, positive)</t>
-  </si>
-  <si>
     <t>0.5, 2</t>
   </si>
   <si>
@@ -91,6 +88,39 @@
   </si>
   <si>
     <t>400k</t>
+  </si>
+  <si>
+    <t>Conv, (128, 128), (64, 128), (1,128)</t>
+  </si>
+  <si>
+    <t>41,3k</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>sample_weight_mode="temporal"</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>added random scaling of input</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>Conv, (128, 128), (64, 128), (32,128),(1,128), elu</t>
+  </si>
+  <si>
+    <t>43,1k</t>
+  </si>
+  <si>
+    <t>Conv, (96, 128), (32, 128), (1,128)</t>
+  </si>
+  <si>
+    <t>very reduced dataset</t>
   </si>
 </sst>
 </file>
@@ -429,17 +459,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -449,7 +479,7 @@
     <col min="12" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -486,8 +516,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>129</v>
       </c>
@@ -498,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>0.44440000000000002</v>
@@ -527,7 +560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>129</v>
       </c>
@@ -535,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>0.49</v>
@@ -557,7 +590,7 @@
         <v>0.48712871287128706</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="1">
         <f>(16*129/2*16+8*8*(129/2-16+1)+8*8*(129/2-16+1-8+1)+4*4*(129/2-16+1-8+1-8+1)+1*30*(129/2-16+1-8+1-8+1-4+1))</f>
@@ -567,7 +600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>384</v>
       </c>
@@ -575,10 +608,10 @@
         <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
         <v>0.34</v>
@@ -597,13 +630,13 @@
         <v>0.1225</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>384</v>
       </c>
@@ -611,10 +644,10 @@
         <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>0.32</v>
@@ -633,21 +666,21 @@
         <v>0.47452631578947374</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="I6" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -661,7 +694,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>384</v>
       </c>
@@ -669,7 +702,7 @@
         <v>128</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1">
         <v>4.62</v>
@@ -691,16 +724,235 @@
         <v>0.70536702767749704</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="I9" s="1" t="e">
+    <row r="9" spans="1:13">
+      <c r="A9" s="1">
+        <v>384</v>
+      </c>
+      <c r="B9" s="1">
+        <v>128</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.63437500000000002</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1">
+        <v>384</v>
+      </c>
+      <c r="B10" s="1">
+        <v>128</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" ref="I10" si="2">2*(G10*H10)/(G10+H10)</f>
+        <v>0.62117647058823533</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="1">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1">
+        <v>384</v>
+      </c>
+      <c r="B11" s="1">
+        <v>128</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" ref="I11" si="3">2*(G11*H11)/(G11+H11)</f>
+        <v>0.55103999999999997</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1">
+        <v>384</v>
+      </c>
+      <c r="B12" s="1">
+        <v>128</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I13" si="4">2*(G12*H12)/(G12+H12)</f>
+        <v>0.62304000000000004</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1">
+        <v>384</v>
+      </c>
+      <c r="B13" s="1">
+        <v>128</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="4"/>
+        <v>0.54120689655172416</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1">
+        <v>384</v>
+      </c>
+      <c r="B14" s="1">
+        <v>128</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.38</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14" si="5">2*(G14*H14)/(G14+H14)</f>
+        <v>0.64850746268656723</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1">
+        <v>20</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged Cached_ADS_Manager and ProjectFilesManager into FileADSManager, and removed caching under the ADSVersion IFileADS's. Fixed bug in Multi_Band_Repair_Marked regarding not skipping markings that are not to be repaired.
</commit_message>
<xml_diff>
--- a/docs/nn results 2020.xlsx
+++ b/docs/nn results 2020.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>INPUTS</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>very reduced dataset</t>
+  </si>
+  <si>
+    <t>28k</t>
+  </si>
+  <si>
+    <t>Conv, (128, 130), (64, 128), (1,128)</t>
+  </si>
+  <si>
+    <t>back to full dataset</t>
+  </si>
+  <si>
+    <t>57,4k</t>
   </si>
 </sst>
 </file>
@@ -459,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -942,17 +954,115 @@
         <v>0.79</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14" si="5">2*(G14*H14)/(G14+H14)</f>
+        <f t="shared" ref="I14:I15" si="5">2*(G14*H14)/(G14+H14)</f>
         <v>0.64850746268656723</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="L14" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M14" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1">
+        <v>384</v>
+      </c>
+      <c r="B15" s="1">
+        <v>128</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.60325203252032522</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="1">
+        <v>45</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
+        <v>384</v>
+      </c>
+      <c r="B16" s="1">
+        <v>128</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16" si="6">2*(G16*H16)/(G16+H16)</f>
+        <v>0.6509615975422427</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="1">
+        <v>20</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>384</v>
+      </c>
+      <c r="B17" s="1">
+        <v>128</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ComputeConfusionMatrixCallback and some pics in the documentation
</commit_message>
<xml_diff>
--- a/docs/nn results 2020.xlsx
+++ b/docs/nn results 2020.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
   <si>
     <t>INPUTS</t>
   </si>
@@ -274,6 +274,34 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Conv(257,96), Conv(1,48), Conv(1,1)=&gt;Output(128,1)</t>
+  </si>
+  <si>
+    <t>1.00, 2.81</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>4096</t>
+  </si>
+  <si>
+    <t>Phase 2 of training</t>
+  </si>
+  <si>
+    <t>Added ReduceLROnPlateau, with init_learn_rate = 0.01, reduction rate = 0.5, patience = 3.
+Phase 1 of training.</t>
+  </si>
+  <si>
+    <t>96000_257_1_20200609-123139.h5</t>
+  </si>
+  <si>
+    <t>29,4k</t>
   </si>
 </sst>
 </file>
@@ -298,7 +326,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -307,21 +335,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -555,7 +568,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -566,7 +581,121 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -582,17 +711,85 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -602,90 +799,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -693,60 +924,122 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,20 +1555,20 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1">
@@ -1671,665 +1964,671 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="10" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="12" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="10" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="37.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="29">
+      <c r="A2" s="18">
         <v>129</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="19">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="19">
         <v>0.43</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="19">
         <v>0.59</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="19">
         <f>2*(G2*H2)/(G2+H2)</f>
         <v>0.49745098039215679</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="19">
         <v>10</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A3" s="27">
+      <c r="A3" s="17">
         <v>129</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="18" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="11">
         <v>0.41</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="11">
         <v>0.6</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I13" si="0">2*(G3*H3)/(G3+H3)</f>
         <v>0.48712871287128706</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="11">
         <v>10</v>
       </c>
-      <c r="L3" s="33"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="25">
+      <c r="A4" s="15">
         <v>384</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="9">
         <v>128</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="9">
         <v>0.73270000000000002</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="9">
         <v>0.68</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="9">
         <f t="shared" si="0"/>
         <v>0.70536702767749704</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="9">
         <v>20</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="26">
+      <c r="A5" s="16">
         <v>384</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="10">
         <v>128</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="17" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="10">
         <v>0.7</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>0.63437500000000002</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="10">
         <v>20</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="26">
+      <c r="A6" s="16">
         <v>384</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="10">
         <v>128</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="10">
         <v>0.48</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="10">
         <v>0.88</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>0.62117647058823533</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="10">
         <v>20</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="26">
+      <c r="A7" s="16">
         <v>384</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="10">
         <v>128</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="10">
         <v>0.41</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="10">
         <v>0.84</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="10">
         <f t="shared" si="0"/>
         <v>0.55103999999999997</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="10">
         <v>20</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="26">
+      <c r="A8" s="16">
         <v>384</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="10">
         <v>128</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="10">
         <v>0.66</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="10">
         <v>0.59</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="10">
         <f t="shared" si="0"/>
         <v>0.62304000000000004</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="10">
         <v>20</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="26">
+      <c r="A9" s="16">
         <v>384</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="10">
         <v>128</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="17" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="10">
         <v>0.43</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="10">
         <v>0.73</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>0.54120689655172416</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="10">
         <v>20</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="26">
+      <c r="A10" s="16">
         <v>384</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="10">
         <v>128</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="10">
         <v>0.79</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="10">
         <f t="shared" si="0"/>
         <v>0.64850746268656723</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="10">
         <v>50</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="27" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="26">
+      <c r="A11" s="16">
         <v>384</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="10">
         <v>128</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="17" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="10">
         <v>0.7</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="10">
         <v>0.53</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="10">
         <f t="shared" si="0"/>
         <v>0.60325203252032522</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="10">
         <v>45</v>
       </c>
-      <c r="L11" s="13"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="26">
+      <c r="A12" s="16">
         <v>384</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="10">
         <v>128</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="10">
         <v>0.65600000000000003</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="10">
         <v>0.64600000000000002</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="10">
         <f t="shared" si="0"/>
         <v>0.6509615975422427</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="10">
         <v>20</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A13" s="27">
+      <c r="A13" s="17">
         <v>384</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="11">
         <v>128</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="18" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="11">
         <v>0.59</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="12">
         <v>0.7</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
         <v>0.64031007751937974</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="11">
         <v>20</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="36"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="36"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="22"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="37"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="37"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="34"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="34"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="34"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="20"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="34"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="35"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="35"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="34"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="34"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C10:C11"/>
@@ -2337,12 +2636,6 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2351,165 +2644,288 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="A1:M4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="3" customWidth="1"/>
-    <col min="7" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="20.5703125" style="3" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" style="2"/>
+    <col min="14" max="14" width="79.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="39" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="M1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="N1" s="33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="I2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="J2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="K2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="9">
+      <c r="L2" s="59"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="28"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="35">
         <v>257</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="53">
         <v>0</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="N3" s="67" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="54">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="71"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="43">
+        <v>257</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="53">
+        <v>0</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="M5" s="45"/>
+      <c r="N5" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="O5" s="72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="54">
+        <v>1</v>
+      </c>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="72"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="64"/>
+      <c r="H7" s="55">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="69" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="54">
+        <v>1</v>
+      </c>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="35">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="H1:K1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>